<commit_message>
ejecucion de codigo unificada
</commit_message>
<xml_diff>
--- a/informe/matriz_v3.xlsx
+++ b/informe/matriz_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nacho\Documents\Github\GIZ\informe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903D4741-2283-4A11-B5A9-D28DF9840F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380B6C9C-E88B-43C6-89A7-C8ED76138520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -628,7 +628,7 @@
   <dimension ref="A1:H534"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>